<commit_message>
Enviando modelagem, script SQL e script Python ATUALIZADOS
</commit_message>
<xml_diff>
--- a/Documentação/Product-Backlog.xlsx
+++ b/Documentação/Product-Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brudn\Desktop\Sprint_1_2semestre\6tracker\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAC4304-A3D9-4977-B42B-2A1A5D2C1081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8964BC26-B370-46C7-AA70-BCCF3126A726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="50">
   <si>
     <t>Requisitos</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>B</t>
-  </si>
-  <si>
-    <t>S5</t>
   </si>
   <si>
     <t>S1</t>
@@ -169,18 +166,6 @@
     <t>Configurar programa de suporte para o site.</t>
   </si>
   <si>
-    <t>(07/08 - 13/08) 6TRACKER - SPRINT 01</t>
-  </si>
-  <si>
-    <t>(14/08 - 20/08) 6TRACKER - SPRINT 02</t>
-  </si>
-  <si>
-    <t>(21/08 - 27/08) 6TRACKER - SPRINT 03</t>
-  </si>
-  <si>
-    <t>(28/08 - 03/09) 6TRACKER- SPRINT 04</t>
-  </si>
-  <si>
     <t>Página onde o cliente poderá cadastrar a unidade em que gerencia e se cadastrar.</t>
   </si>
   <si>
@@ -200,6 +185,12 @@
   </si>
   <si>
     <t>Criar banco de dados do projeto.</t>
+  </si>
+  <si>
+    <t>6TRACKER - SPRINT 02</t>
+  </si>
+  <si>
+    <t>6RACKER - SPRINT 01</t>
   </si>
 </sst>
 </file>
@@ -269,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,8 +279,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -410,19 +407,6 @@
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
@@ -453,11 +437,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -501,38 +509,50 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -856,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -877,7 +897,7 @@
   <sheetData>
     <row r="2" spans="1:12" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -889,7 +909,7 @@
     </row>
     <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -948,7 +968,7 @@
         <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -956,13 +976,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
@@ -974,7 +994,7 @@
         <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -982,7 +1002,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>9</v>
@@ -1000,16 +1020,16 @@
         <v>29</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>9</v>
@@ -1027,7 +1047,7 @@
         <v>29</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="L9" s="7"/>
     </row>
@@ -1054,15 +1074,15 @@
         <v>23</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>9</v>
@@ -1080,15 +1100,15 @@
         <v>23</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>9</v>
@@ -1106,15 +1126,15 @@
         <v>23</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>9</v>
@@ -1158,7 +1178,7 @@
         <v>23</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L14" s="7"/>
     </row>
@@ -1167,7 +1187,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>9</v>
@@ -1185,12 +1205,12 @@
         <v>29</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>18</v>
@@ -1199,7 +1219,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>11</v>
@@ -1211,7 +1231,7 @@
         <v>29</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1222,7 +1242,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>13</v>
@@ -1242,7 +1262,7 @@
     </row>
     <row r="19" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
@@ -1254,7 +1274,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -1295,7 +1315,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>9</v>
@@ -1313,406 +1333,388 @@
         <v>29</v>
       </c>
       <c r="H23" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1">
+        <v>5</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
+      <c r="E25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1">
+        <v>5</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2">
+        <v>8</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="B27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="2">
+        <v>8</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2">
+        <v>8</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B32" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C32" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F32" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G32" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H32" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="12">
+        <v>5</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="2">
         <v>8</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="1">
+      <c r="G34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="23">
+        <v>13</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="26">
         <v>5</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="G36" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="1">
-        <v>5</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="12">
-        <v>5</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="2">
-        <v>8</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="2">
-        <v>8</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="23"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="2">
-        <v>8</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F37" s="2">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="12">
-        <v>5</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I40" s="7"/>
-    </row>
-    <row r="41" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="2">
-        <v>8</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="2">
-        <v>8</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="27"/>
+    </row>
+    <row r="41" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="28"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="14"/>
@@ -1728,14 +1730,13 @@
       <c r="C51" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A34:H34"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A31:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>